<commit_message>
texture fix (missing blockstates)
</commit_message>
<xml_diff>
--- a/docu_plan.xlsx
+++ b/docu_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\MC-modding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC1ED7B-E705-40B9-9121-54D7CDF29752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE1F090-BF3C-4D78-8B5B-79E611191722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blocks" sheetId="1" r:id="rId1"/>
@@ -505,8 +505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +538,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C4" t="str">
@@ -547,7 +547,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C5" t="str">
@@ -556,7 +556,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C6" t="str">
@@ -565,7 +565,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C7" t="str">
@@ -574,7 +574,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="str">
@@ -695,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
renaming and new tool
</commit_message>
<xml_diff>
--- a/docu_plan.xlsx
+++ b/docu_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\MC-modding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7A486B-7252-4C30-9230-D4FE3F8215A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277154F7-70DC-45AA-A8F5-8B3C77A1E8B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="10245" windowHeight="7800" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="5085" windowHeight="7800" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blocks" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Blocks</t>
   </si>
@@ -72,9 +72,6 @@
     <t>smelted_aare</t>
   </si>
   <si>
-    <t>-&gt; aare_pickaxe</t>
-  </si>
-  <si>
     <t>Recipes</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>aaronic_multitool</t>
+  </si>
+  <si>
+    <t>&lt;-</t>
   </si>
 </sst>
 </file>
@@ -215,9 +215,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,7 +521,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -544,8 +544,8 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>20</v>
+      <c r="A4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C4" t="str">
         <f>UPPER(A4)</f>
@@ -553,8 +553,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>32</v>
+      <c r="A5" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ref="C5:C8" si="1">UPPER(A5)</f>
@@ -562,8 +562,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>33</v>
+      <c r="A6" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
@@ -571,8 +571,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>27</v>
+      <c r="A7" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
@@ -580,8 +580,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>28</v>
+      <c r="A8" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
@@ -629,7 +629,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="str">
@@ -661,8 +661,8 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>22</v>
+      <c r="A5" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -670,8 +670,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>34</v>
+      <c r="A6" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -686,34 +686,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>35</v>
+      <c r="D2" t="str">
+        <f>UPPER(A2)</f>
+        <v>AARE_PICKAXE</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="str">
+        <f>UPPER(A3)</f>
+        <v>AARONIC_MULTITOOL</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -728,8 +738,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>10</v>
+      <c r="A1" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -737,18 +747,18 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -759,7 +769,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -770,10 +780,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -781,7 +791,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -789,13 +799,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -814,8 +824,8 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
+      <c r="A1" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,10 +833,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -848,13 +858,13 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>16</v>
+      <c r="A1" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">
@@ -879,16 +889,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>18</v>
+      <c r="A1" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -896,24 +906,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">
@@ -938,48 +948,48 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>19</v>
+      <c r="A1" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>